<commit_message>
Model Deploymnet with Streamlit
</commit_message>
<xml_diff>
--- a/Web-Scraping/stb.xlsx
+++ b/Web-Scraping/stb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B375"/>
+  <dimension ref="A1:B372"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -726,7 +726,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/flipkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-g-star-raw-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-g-star-raw-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-gas-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-gas-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/gini-&amp;-jony-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/gini-&amp;-jony-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/giva-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/giva-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/grt-jewellers-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/grt-jewellers-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-hamleys-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-hamleys-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/helios-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/helios-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hidesign-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hidesign-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hush-puppies-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hush-puppies-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/jack-&amp;-jones-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/jack-&amp;-jones-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kalyan-diamond-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kalyan-diamond-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kalyan-gold-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kalyan-gold-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ketan-diamonds-gold-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ketan-diamonds-gold-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kiehls-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kiehls-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/levis-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/levis-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/max-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -936,7 +936,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/max-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/max-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/max-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-mothercare-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-mothercare-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/myntra-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/myntra-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-fashion-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-fashion-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-man-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -996,7 +996,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-man-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/only-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/only-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pantaloons-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pantaloons-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pc-jeweller-diamond-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pc-jeweller-diamond-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pc-jeweller-gold-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pc-jeweller-gold-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/puma-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/puma-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/relaxo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/relaxo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-jewels-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-jewels-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-point-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-point-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-trends-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-trends-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-trends-footwear-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-trends-footwear-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card--replay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card--replay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/shiv-naresh-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/shiv-naresh-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/shoppers-stop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/shoppers-stop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/skechers-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/skechers-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/skinn-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/skinn-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/spencers-retail-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/spencers-retail-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-steve-madden-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-steve-madden-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-superdry-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-superdry-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-luxury-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-luxury-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-palette-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-palette-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tego-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tego-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-body-shop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-body-shop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-man-company-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-man-company-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-raymond-shop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-raymond-shop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/titan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/titan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/titan-minimals-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/titan-minimals-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/unlimited-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/unlimited-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/v-mart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/v-mart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/veromoda-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/veromoda-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/w-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/w-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/wildcraft-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/wildcraft-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/william-penn-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/william-penn-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/woggles-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/woggles-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/woodland-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/woodland-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/intermiles-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/intermiles-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ixigo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ixigo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ola-cabs-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ola-cabs-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/points-for-people-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/points-for-people-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/samsonite-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/samsonite-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/taj-hotels-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/taj-hotels-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/uber-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/uber-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/yatra.com-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/yatra.com-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/archies-gallery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/archies-gallery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/aurelia-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/aurelia-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/balenzia-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/balenzia-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bata-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bata-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bewakoof-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bewakoof-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/beyoung-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/beyoung-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/candere-diamond-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/candere-diamond-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/candere-gold-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/candere-gold-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-gold-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-gold-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-silver-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-silver-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ferns-n-petals-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ferns-n-petals-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/flower-aura-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/flipkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/flower-aura-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/home-centre-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/igp-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-centre-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/igp-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/max-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/muthoot-gold-voucher-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/max-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mxplayer-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/muthoot-gold-voucher-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/myntra-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mxplayer-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/myupchar-medicines-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/myntra-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/myupchar-medicines-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-fashion-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/nykaa-man-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-fashion-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ola-cabs-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/nykaa-man-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/organic-india-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ola-cabs-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/points-for-people-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/organic-india-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pvr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/points-for-people-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/renee-cosmetics-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pvr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/samsonite-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/renee-cosmetics-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/samsonite-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/skullcandy-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/smile-foundation-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/skullcandy-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/sonyliv-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/smile-foundation-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/superbottoms-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/sonyliv-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/swiggy-gv-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/superbottoms-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/swiss-beauty-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/swiggy-gv-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/swiss-beauty-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-luxury-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2256,7 +2256,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-palette-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-luxury-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tego-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tata-cliq-palette-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-skin-story-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tego-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/veridicus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-skin-story-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/vrott-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/veridicus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/woggles-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/vrott-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/wonderchef-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/woggles-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/zomato-gift-card-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/wonderchef-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/zomato-gift-card-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/et-prime-subscription-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/et-prime-subscription-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mxplayer-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pvr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mxplayer-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/sonyliv-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pvr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/vrott-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/sonyliv-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/zee5-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/vrott-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/zee5-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/barbeque-nation-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/baskin-robbins-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/barbeque-nation-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/beer-cafe-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/baskin-robbins-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/cafe-delhi-heights-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/beer-cafe-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/cafe-delhi-heights-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/costa-coffee-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/dominos-pizza-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/costa-coffee-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kfc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/dominos-pizza-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/machaan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kfc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mainland-china-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/machaan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/oh!-calcutta-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mainland-china-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/pizza-hut-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/oh!-calcutta-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/sigree-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/pizza-hut-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/sweet-bengal-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/sigree-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/swiggy-gv-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/sweet-bengal-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/tgif-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/swiggy-gv-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/wonderchef-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/tgif-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/zomato-gift-card-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/wonderchef-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/zomato-gift-card-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-prime-membership-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-prime-membership-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/american-tourister-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/archies-gallery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-armani-exchange-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/archies-gallery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/arrow-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-armani-exchange-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/arrow-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/aurelia-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/assembly-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/aurelia-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/balenzia-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bakingo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/barbeque-nation-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/balenzia-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/baskin-robbins-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/barbeque-nation-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bata-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/baskin-robbins-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/beer-cafe-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bata-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bewakoof-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/beer-cafe-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/beyoung-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bewakoof-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/beyoung-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bluestone-diamond-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bluestone-gold-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bluestone-diamond-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bobbi-brown-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bluestone-gold-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bobbi-brown-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-brooks-brothers-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/braingymjr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/cafe-delhi-heights-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-brooks-brothers-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/campus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/cafe-delhi-heights-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/candere-diamond-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/campus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/candere-gold-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/candere-diamond-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/celio-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/candere-gold-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/celio-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/chumbak-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/chicago-pizza-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/chumbak-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/costa-coffee-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/costa-coffee-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/discovery-plus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/dominos-pizza-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/docubay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/dpauls-travel-tours-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/dominos-pizza-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card--dune-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3106,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/dpauls-travel-tours-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/elleven-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card--dune-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/estele-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/elleven-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/et-prime-subscription-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/estele-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-gold-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/et-prime-subscription-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-silver-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-gold-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/euphoria-jewellery-silver-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fabindia-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3176,7 +3176,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fab-hotels-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fashion-factory-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fabindia-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fastrack-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fashion-factory-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fastrack-bags-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fastrack-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ferns-n-petals-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fastrack-bags-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3226,7 +3226,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ferns-n-petals-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/flower-aura-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/flipkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-g-star-raw-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/flower-aura-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-gas-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/freecultr-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/gini-&amp;-jony-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-g-star-raw-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/giva-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-gas-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/gini-&amp;-jony-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/grt-jewellers-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/giva-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-hamleys-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/grt-jewellers-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-–-hamleys-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/helios-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hidesign-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/helios-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/home-stop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hidesign-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hush-puppies-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hoichoi-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/igp-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-centre-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/intermiles-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-stop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hush-puppies-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ixigo-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/igp-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/jack-&amp;-jones-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/intermiles-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/irctc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kalyan-diamond-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ixigo-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kalyan-gold-jewellery-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/jack-&amp;-jones-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kama-ayurveda-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/jockey-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/ketan-diamonds-gold-coin-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kalyan-diamond-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kfc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kalyan-gold-jewellery-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kiehls-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kama-ayurveda-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/levis-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3546,7 +3546,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/ketan-diamonds-gold-coin-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kfc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kiehls-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/levis-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/machaan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/lifestyle-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mainland-china-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/luxe-gift-card-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/machaan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mainland-china-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/max-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-holiday-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/max-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/makemytrip-hotel-e-pay-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-fresh-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/bigbasket-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/home-centre-online-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/home-stop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-centre-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/more-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-centre-online-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/prestige-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/home-stop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-jio-mart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/more-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/prestige-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-point-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-jio-mart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/sleepwell-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/spencers-retail-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-smart-point-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/unlimited-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3796,7 +3796,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/sleepwell-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/v-mart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/spencers-retail-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/unlimited-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/v-mart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/apollo-pharmacy-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/auric-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/decathlon-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/finusmart-easy-cash-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/fitpass-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/gnc-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthians-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/kama-ayurveda-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthifyme-smart-plan-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/healthkart-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/kama-ayurveda-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/myupchar-medicines-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/love-beauty-planet-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/netmeds-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/mamaearth-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/organic-india-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/myupchar-medicines-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/renee-cosmetics-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/netmeds-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/organic-india-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/smile-foundation-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/renee-cosmetics-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/superbottoms-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/simple-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/swiss-beauty-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/smile-foundation-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-body-shop-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/superbottoms-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/the-skin-story-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/swiss-beauty-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/truefitt-hill-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-body-shop-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/veridicus-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/the-skin-story-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/truefitt-hill-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/veridicus-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/amazon-shopping-voucher-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/avast-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/black-decker-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/corseca-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/croma-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-digital-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/daily-objects-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/reliance-my-jio-store-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>https://www.gyftr.com/sc-instavouchers/hammer-gift-vouchers</t>
+          <t>https://www.gyftr.com/sc-instavouchers/skullcandy-gift-vouchers</t>
         </is>
       </c>
     </row>
@@ -4145,36 +4145,6 @@
         <v>370</v>
       </c>
       <c r="B372" t="inlineStr">
-        <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-digital-gift-vouchers</t>
-        </is>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" s="1" t="n">
-        <v>371</v>
-      </c>
-      <c r="B373" t="inlineStr">
-        <is>
-          <t>https://www.gyftr.com/sc-instavouchers/reliance-my-jio-store-gift-vouchers</t>
-        </is>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" s="1" t="n">
-        <v>372</v>
-      </c>
-      <c r="B374" t="inlineStr">
-        <is>
-          <t>https://www.gyftr.com/sc-instavouchers/skullcandy-gift-vouchers</t>
-        </is>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" s="1" t="n">
-        <v>373</v>
-      </c>
-      <c r="B375" t="inlineStr">
         <is>
           <t>https://www.gyftr.com/sc-instavouchers/vijay-sales-gift-vouchers</t>
         </is>

</xml_diff>